<commit_message>
add DataBase + getArticleFemme + Homme
</commit_message>
<xml_diff>
--- a/Plan projet/RoadMap.xlsx
+++ b/Plan projet/RoadMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kween\Bureau\Ynov\B1 INFO\SEMESTRE 2\Module_CHALLENGE-JS\PROJET\Plan projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BACCD-655F-46D6-AB70-3C09E952E8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E84425C-C36F-4CC7-8B33-D84FE6B58E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>BOUTIQUE CARACTERISTIQUES</t>
   </si>
@@ -129,13 +129,19 @@
     <t>NOM DES TACHES</t>
   </si>
   <si>
-    <t>DIOR mais a lenvers RIOD</t>
-  </si>
-  <si>
     <t>Logo dispo sur Figma</t>
   </si>
   <si>
     <t>KANTIN / ARTHUR</t>
+  </si>
+  <si>
+    <t>UX &amp; UI OK</t>
+  </si>
+  <si>
+    <t>ROID inspiration de dior</t>
+  </si>
+  <si>
+    <t>Maquettes dispo sur Figma</t>
   </si>
 </sst>
 </file>
@@ -435,17 +441,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,49 +501,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,7 +885,7 @@
   <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="P12" sqref="P12:Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -889,786 +895,790 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="12" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
     </row>
     <row r="2" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
       <c r="AD2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="31" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
       <c r="AD3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="31" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
       <c r="AD4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="31" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="31" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
     </row>
     <row r="7" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
       <c r="AD7" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="21" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="31" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
       <c r="AD8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="21" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
       <c r="AD9" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
       <c r="AD10" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="31" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
     </row>
     <row r="12" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="31" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
     </row>
     <row r="13" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="31" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
     </row>
     <row r="15" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="31" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
     </row>
     <row r="16" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="31" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
     </row>
     <row r="17" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="31" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
     </row>
     <row r="18" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="31" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
     </row>
     <row r="19" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="31" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
     </row>
     <row r="20" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="31" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
     </row>
     <row r="21" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="31" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="10"/>
-      <c r="Y21" s="10"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
     </row>
     <row r="22" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="31" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
     </row>
     <row r="23" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="31" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
     </row>
     <row r="24" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="31" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
     </row>
     <row r="25" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="8"/>
@@ -1683,55 +1693,41 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="K9:O9"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="K15:O15"/>
-    <mergeCell ref="K16:O16"/>
-    <mergeCell ref="K17:O17"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="K10:O10"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="P12:Y12"/>
+    <mergeCell ref="P14:Y14"/>
+    <mergeCell ref="P15:Y15"/>
+    <mergeCell ref="P16:Y16"/>
+    <mergeCell ref="P13:T13"/>
+    <mergeCell ref="U13:Y13"/>
+    <mergeCell ref="P22:Y22"/>
+    <mergeCell ref="P23:Y23"/>
+    <mergeCell ref="P24:Y24"/>
+    <mergeCell ref="P17:Y17"/>
+    <mergeCell ref="P18:Y18"/>
+    <mergeCell ref="P19:Y19"/>
+    <mergeCell ref="P20:Y20"/>
+    <mergeCell ref="P21:Y21"/>
+    <mergeCell ref="P11:Y11"/>
+    <mergeCell ref="P1:Y1"/>
+    <mergeCell ref="P3:Y3"/>
+    <mergeCell ref="P4:Y4"/>
+    <mergeCell ref="P5:Y5"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="U10:Y10"/>
+    <mergeCell ref="P6:Y6"/>
+    <mergeCell ref="P8:Y8"/>
+    <mergeCell ref="P9:Y9"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="U7:Y7"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A21:E21"/>
@@ -1748,41 +1744,55 @@
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="P11:Y11"/>
-    <mergeCell ref="P1:Y1"/>
-    <mergeCell ref="P3:Y3"/>
-    <mergeCell ref="P4:Y4"/>
-    <mergeCell ref="P5:Y5"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="U10:Y10"/>
-    <mergeCell ref="P6:Y6"/>
-    <mergeCell ref="P8:Y8"/>
-    <mergeCell ref="P9:Y9"/>
-    <mergeCell ref="P7:T7"/>
-    <mergeCell ref="U7:Y7"/>
-    <mergeCell ref="P22:Y22"/>
-    <mergeCell ref="P23:Y23"/>
-    <mergeCell ref="P24:Y24"/>
-    <mergeCell ref="P17:Y17"/>
-    <mergeCell ref="P18:Y18"/>
-    <mergeCell ref="P19:Y19"/>
-    <mergeCell ref="P20:Y20"/>
-    <mergeCell ref="P21:Y21"/>
-    <mergeCell ref="P12:Y12"/>
-    <mergeCell ref="P14:Y14"/>
-    <mergeCell ref="P15:Y15"/>
-    <mergeCell ref="P16:Y16"/>
-    <mergeCell ref="P13:T13"/>
-    <mergeCell ref="U13:Y13"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="K9:O9"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="K18:O18"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="K24:O24"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K14:O24 K8:O9 K3:O6 K11:O12" xr:uid="{546E0733-B499-451F-8417-27B03B85F6A9}">

</xml_diff>